<commit_message>
For Tim, for augmentation. READ FILE FIRST
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results-new.xlsx
+++ b/Baseline-experimental-results-new.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Dataset</t>
   </si>
@@ -110,6 +110,9 @@
   <si>
     <t>11 (71 min, PER)</t>
   </si>
+  <si>
+    <t>14 (56 min, PER)</t>
+  </si>
 </sst>
 </file>
 
@@ -120,7 +123,7 @@
     <numFmt numFmtId="164" formatCode="0.000000%"/>
     <numFmt numFmtId="165" formatCode="0.00000%"/>
     <numFmt numFmtId="166" formatCode="0.0000%"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -171,12 +174,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="2" builtinId="3"/>
@@ -452,7 +455,7 @@
                   <c:v>0.98684000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.43049999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,7 +536,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
-          <c:min val="0.75000000000000011"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2518,7 +2520,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,18 +2533,18 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2580,6 +2582,9 @@
       <c r="E3">
         <v>196110</v>
       </c>
+      <c r="G3">
+        <v>91580</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2594,6 +2599,9 @@
       <c r="E4">
         <v>49027</v>
       </c>
+      <c r="G4">
+        <v>22895</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2608,6 +2616,9 @@
       <c r="E5">
         <v>589</v>
       </c>
+      <c r="G5">
+        <v>27646</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2622,6 +2633,9 @@
       <c r="E6" t="s">
         <v>27</v>
       </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2637,6 +2651,10 @@
       <c r="E7" s="1">
         <f>1-E8</f>
         <v>1.315999999999995E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f>1-G8</f>
+        <v>0.56950000000000001</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -2654,7 +2672,9 @@
       <c r="E8" s="1">
         <v>0.98684000000000005</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>0.43049999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -2700,7 +2720,7 @@
       </c>
       <c r="C13" s="2">
         <f>G8</f>
-        <v>0</v>
+        <v>0.43049999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -2736,18 +2756,18 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2776,7 +2796,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>0.72683469024386704</v>
       </c>
       <c r="C3" s="5"/>
@@ -2790,7 +2810,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>0.79985174194276498</v>
       </c>
       <c r="C4" s="5"/>
@@ -2803,7 +2823,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>0.838769451479632</v>
       </c>
       <c r="C5" s="5"/>
@@ -2816,7 +2836,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>0.87027427286815395</v>
       </c>
       <c r="C6" s="5"/>
@@ -2829,7 +2849,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>0.76723498675980495</v>
       </c>
       <c r="C7" s="5"/>
@@ -2842,7 +2862,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>0.69940697112907002</v>
       </c>
       <c r="C8" s="5"/>
@@ -2855,7 +2875,7 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>0.87546330129243</v>
       </c>
       <c r="C9" s="5"/>
@@ -2868,7 +2888,7 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>0.86582653592302605</v>
       </c>
       <c r="C10" s="5"/>
@@ -2881,7 +2901,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>0.79948109295564296</v>
       </c>
       <c r="C11" s="5"/>
@@ -2894,7 +2914,7 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>0.57709414641710399</v>
       </c>
       <c r="C12" s="5"/>
@@ -2937,27 +2957,27 @@
       <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <f>_xlfn.STDEV.P(B3:B12)</f>
         <v>8.9146450645818373E-2</v>
       </c>
-      <c r="C14" s="13" t="e">
+      <c r="C14" s="12" t="e">
         <f>_xlfn.STDEV.P(C3:C12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D14" s="13" t="e">
+      <c r="D14" s="12" t="e">
         <f t="shared" ref="D14:G14" si="1">_xlfn.STDEV.P(D3:D12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E14" s="13" t="e">
+      <c r="E14" s="12" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F14" s="13" t="e">
+      <c r="F14" s="12" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G14" s="13" t="e">
+      <c r="G14" s="12" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2967,27 +2987,27 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <f>B14/SQRT(10)</f>
         <v>2.8190582936057442E-2</v>
       </c>
-      <c r="C15" s="13" t="e">
+      <c r="C15" s="12" t="e">
         <f>C14/SQRT(10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="13" t="e">
+      <c r="D15" s="12" t="e">
         <f t="shared" ref="D15:G15" si="2">D14/SQRT(10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E15" s="13" t="e">
+      <c r="E15" s="12" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F15" s="13" t="e">
+      <c r="F15" s="12" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G15" s="13" t="e">
+      <c r="G15" s="12" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
All functions are now in preprocessing
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results-new.xlsx
+++ b/Baseline-experimental-results-new.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Dataset</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>14 (56 min, PER)</t>
+  </si>
+  <si>
+    <t>CNN-1</t>
+  </si>
+  <si>
+    <t>CNN-2</t>
+  </si>
+  <si>
+    <t>CNN2-nodrop</t>
+  </si>
+  <si>
+    <t>CNN-2-nodrop</t>
+  </si>
+  <si>
+    <t>Extended_bin_Aug</t>
+  </si>
+  <si>
+    <t>CNN1</t>
   </si>
 </sst>
 </file>
@@ -2142,16 +2160,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>814387</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>738187</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2517,19 +2535,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2537,16 +2568,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2557,19 +2597,46 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2579,14 +2646,14 @@
       <c r="C3">
         <v>21584</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>196110</v>
       </c>
-      <c r="G3">
+      <c r="M3">
         <v>91580</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2596,14 +2663,14 @@
       <c r="C4">
         <v>5396</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>49027</v>
       </c>
-      <c r="G4">
+      <c r="M4">
         <v>22895</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2613,14 +2680,14 @@
       <c r="C5">
         <v>589</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>589</v>
       </c>
-      <c r="G5">
+      <c r="M5">
         <v>27646</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2630,14 +2697,14 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
+      <c r="M6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2649,17 +2716,23 @@
         <f>1-C8</f>
         <v>9.4514499999999946E-2</v>
       </c>
-      <c r="E7" s="1">
-        <f>1-E8</f>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1">
+        <f>1-H8</f>
         <v>1.315999999999995E-2</v>
       </c>
-      <c r="G7" s="2">
-        <f>1-G8</f>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="M7" s="2">
+        <f>1-M8</f>
         <v>0.56950000000000001</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2669,22 +2742,37 @@
       <c r="C8" s="1">
         <v>0.90548550000000005</v>
       </c>
-      <c r="E8" s="1">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="1">
         <v>0.98684000000000005</v>
       </c>
-      <c r="G8" s="1">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="M8" s="1">
         <v>0.43049999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -2696,38 +2784,52 @@
         <f>C8</f>
         <v>0.90548550000000005</v>
       </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B12">
-        <f>D8</f>
+        <f>G8</f>
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f>E8</f>
+        <f>H8</f>
         <v>0.98684000000000005</v>
       </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <f>F8</f>
+        <f>L8</f>
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <f>G8</f>
+        <f>M8</f>
         <v>0.43049999999999999</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fast changes, ready for more classifier testing
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results-new.xlsx
+++ b/Baseline-experimental-results-new.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Dataset</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Bin_augmented</t>
   </si>
   <si>
-    <t>Bin_Augmented</t>
-  </si>
-  <si>
     <t>128_extended_bin</t>
   </si>
   <si>
@@ -126,10 +123,28 @@
     <t>CNN-2-nodrop</t>
   </si>
   <si>
-    <t>Extended_bin_Aug</t>
-  </si>
-  <si>
     <t>CNN1</t>
+  </si>
+  <si>
+    <t>19 (101 min, PER)</t>
+  </si>
+  <si>
+    <t>29 ( 71 min, PER)</t>
+  </si>
+  <si>
+    <t>11 (25 min, PER)</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Original_Augmented</t>
+  </si>
+  <si>
+    <t>Extended</t>
+  </si>
+  <si>
+    <t>Extended_Augmented</t>
   </si>
 </sst>
 </file>
@@ -181,7 +196,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,6 +210,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -231,6 +249,61 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>Network accuracy per dataset</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -305,14 +378,13 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:ln w="9525">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -326,13 +398,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Original_bin</c:v>
+                  <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Bin_Augmented</c:v>
+                  <c:v>Original_Augmented</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Extended_bin</c:v>
+                  <c:v>Extended</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -428,14 +500,13 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                    <a:ln w="9525">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -449,13 +520,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Original_bin</c:v>
+                  <c:v>Original</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Bin_Augmented</c:v>
+                  <c:v>Original_Augmented</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Extended_bin</c:v>
+                  <c:v>Extended</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -481,6 +552,354 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2A99-4E4C-A4D6-42531CE76C50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>new_results!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CNN-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>new_results!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original_Augmented</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extended</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>new_results!$D$11:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.95789999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA05-47B9-BD12-1D3A1F04AABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>new_results!$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CNN-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>new_results!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original_Augmented</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extended</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>new_results!$E$11:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.97219999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BA05-47B9-BD12-1D3A1F04AABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>new_results!$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CNN-2-nodrop</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>new_results!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original_Augmented</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extended</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>new_results!$F$11:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BA05-47B9-BD12-1D3A1F04AABE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -493,8 +912,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="199"/>
         <c:axId val="475002800"/>
         <c:axId val="475003128"/>
       </c:barChart>
@@ -527,7 +945,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -554,6 +972,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
+          <c:min val="0.75000000000000011"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -571,6 +990,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1151,6 +1584,506 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="212">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1653,509 +2586,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2166,7 +2596,7 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -2535,108 +2965,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
       <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="N1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2646,14 +3079,23 @@
       <c r="C3">
         <v>21584</v>
       </c>
-      <c r="H3">
+      <c r="D3">
+        <v>21584</v>
+      </c>
+      <c r="E3">
+        <v>21584</v>
+      </c>
+      <c r="F3">
+        <v>21584</v>
+      </c>
+      <c r="I3">
         <v>196110</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>91580</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2663,14 +3105,23 @@
       <c r="C4">
         <v>5396</v>
       </c>
-      <c r="H4">
+      <c r="D4">
+        <v>5396</v>
+      </c>
+      <c r="E4">
+        <v>5396</v>
+      </c>
+      <c r="F4">
+        <v>5396</v>
+      </c>
+      <c r="I4">
         <v>49027</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>22895</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2680,31 +3131,49 @@
       <c r="C5">
         <v>589</v>
       </c>
-      <c r="H5">
+      <c r="D5">
         <v>589</v>
       </c>
-      <c r="M5">
+      <c r="E5">
+        <v>589</v>
+      </c>
+      <c r="F5">
+        <v>589</v>
+      </c>
+      <c r="I5">
+        <v>589</v>
+      </c>
+      <c r="O5">
         <v>27646</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="O6" t="s">
         <v>27</v>
       </c>
-      <c r="M6" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2716,23 +3185,62 @@
         <f>1-C8</f>
         <v>9.4514499999999946E-2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:R7" si="0">1-D8</f>
+        <v>4.2100000000000026E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7800000000000047E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5400000000000005E-2</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1">
-        <f>1-H8</f>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
         <v>1.315999999999995E-2</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="M7" s="2">
-        <f>1-M8</f>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="0"/>
         <v>0.56950000000000001</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="P7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2742,39 +3250,47 @@
       <c r="C8" s="1">
         <v>0.90548550000000005</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="H8" s="1">
+      <c r="D8" s="1">
+        <v>0.95789999999999997</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.9446</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="I8" s="1">
         <v>0.98684000000000005</v>
       </c>
-      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="M8" s="1">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="O8" s="1">
         <v>0.43049999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2">
         <f>B8</f>
@@ -2784,52 +3300,64 @@
         <f>C8</f>
         <v>0.90548550000000005</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="2">
+        <f>D8</f>
+        <v>0.95789999999999997</v>
+      </c>
+      <c r="E11" s="2">
+        <f>E8</f>
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="F11" s="2">
+        <f>F8</f>
+        <v>0.9446</v>
+      </c>
+      <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B12">
-        <f>G8</f>
+        <f>H8</f>
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f>H8</f>
+        <f>I8</f>
         <v>0.98684000000000005</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <f>L8</f>
+        <f>N8</f>
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <f>M8</f>
+        <f>O8</f>
         <v>0.43049999999999999</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="N1:R1"/>
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2841,13 +3369,13 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" customWidth="1"/>
@@ -2858,40 +3386,40 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3117,18 +3645,18 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8">
         <f>B13</f>
@@ -3143,7 +3671,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="8" t="e">
         <f>D13</f>
@@ -3158,7 +3686,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="8" t="e">
         <f>F13</f>

</xml_diff>

<commit_message>
FINAL PREPROCESSING, DONE NOW!
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results-new.xlsx
+++ b/Baseline-experimental-results-new.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Oosterhuis\Documents\GitHub\HWR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rogier\Documents\Studie\HWR_own\HWR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="new_results" sheetId="3" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Base-CNN</t>
   </si>
   <si>
-    <t>16 ( 4 min, ROG))</t>
-  </si>
-  <si>
     <t>11 (71 min, PER)</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Extended_Augmented</t>
   </si>
   <si>
-    <t>8 (10 min, PER)</t>
-  </si>
-  <si>
     <t>CNN_6conv_1</t>
   </si>
   <si>
@@ -163,6 +157,12 @@
   </si>
   <si>
     <t>7 (t=2:43, 10 folds, PER)</t>
+  </si>
+  <si>
+    <t>8 (100 min, 10-fold, PER)</t>
+  </si>
+  <si>
+    <t>16 ( 4 min, 10-fold, ROG))</t>
   </si>
 </sst>
 </file>
@@ -170,11 +170,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.000000%"/>
-    <numFmt numFmtId="166" formatCode="0.00000%"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.000000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -212,20 +212,20 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,7 +321,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -383,7 +383,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -505,7 +505,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -627,7 +627,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -743,7 +743,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -862,7 +862,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -924,6 +924,125 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BA05-47B9-BD12-1D3A1F04AABE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>new_results!$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CNN_6conv_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="nl-NL"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>new_results!$A$11:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Original</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Original_Augmented</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extended</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>new_results!$G$11:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.9607</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19650000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC2C-4C21-9F48-8695F9891C37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -981,7 +1100,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475003128"/>
@@ -1055,7 +1174,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475002800"/>
@@ -1097,7 +1216,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1127,7 +1246,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1385,7 +1504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438729832"/>
@@ -1446,7 +1565,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438729504"/>
@@ -1488,7 +1607,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1518,7 +1637,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2990,32 +3109,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="13.33203125" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" customWidth="1"/>
-    <col min="19" max="19" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3049,7 +3173,7 @@
       <c r="W1" s="14"/>
       <c r="X1" s="14"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3060,19 +3184,19 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
         <v>20</v>
@@ -3081,19 +3205,19 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
       <c r="O2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R2" t="s">
         <v>20</v>
@@ -3102,22 +3226,22 @@
         <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" t="s">
         <v>29</v>
       </c>
-      <c r="V2" t="s">
-        <v>30</v>
-      </c>
       <c r="W2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="X2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3152,7 +3276,7 @@
         <v>91580</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3187,7 +3311,7 @@
         <v>22895</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3222,45 +3346,45 @@
         <v>27646</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
       <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s">
         <v>43</v>
       </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="S6" t="s">
         <v>26</v>
       </c>
-      <c r="R6" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" t="s">
-        <v>27</v>
-      </c>
       <c r="W6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3288,58 +3412,70 @@
         <f>1-G8</f>
         <v>3.9300000000000002E-2</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7:X7" si="1">1-H8</f>
+        <v>1</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8199999999999918E-2</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.315999999999995E-2</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="O7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.91739999999999999</v>
       </c>
       <c r="S7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.56950000000000001</v>
       </c>
       <c r="T7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.36809999999999998</v>
       </c>
       <c r="V7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="W7" s="1">
-        <f>1-W8</f>
+        <f t="shared" si="1"/>
         <v>0.80349999999999999</v>
       </c>
-      <c r="X7" s="1"/>
+      <c r="X7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3388,7 +3524,7 @@
         <v>0.19650000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -3396,55 +3532,55 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2">
-        <f>B8</f>
+        <f t="shared" ref="B11:G11" si="2">B8</f>
         <v>0.78200000000000003</v>
       </c>
       <c r="C11" s="2">
-        <f>C8</f>
+        <f t="shared" si="2"/>
         <v>0.90548550000000005</v>
       </c>
       <c r="D11" s="2">
-        <f>D8</f>
+        <f t="shared" si="2"/>
         <v>0.95789999999999997</v>
       </c>
       <c r="E11" s="2">
-        <f>E8</f>
+        <f t="shared" si="2"/>
         <v>0.97219999999999995</v>
       </c>
       <c r="F11" s="2">
-        <f>F8</f>
+        <f t="shared" si="2"/>
         <v>0.9446</v>
       </c>
       <c r="G11" s="2">
-        <f>G8</f>
+        <f t="shared" si="2"/>
         <v>0.9607</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="2">
         <f>J8</f>
@@ -3461,9 +3597,9 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2">
         <f>R8</f>
@@ -3486,9 +3622,9 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3510,17 +3646,17 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3537,7 +3673,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3560,7 +3696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3576,7 +3712,7 @@
       <c r="G3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3591,7 +3727,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3606,7 +3742,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3621,7 +3757,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3636,7 +3772,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3651,7 +3787,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3666,7 +3802,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3681,7 +3817,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3696,7 +3832,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3711,7 +3847,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3741,7 +3877,7 @@
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -3771,7 +3907,7 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3801,7 +3937,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3812,7 +3948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3827,7 +3963,7 @@
       <c r="D19" s="9"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3842,7 +3978,7 @@
       <c r="D20" s="9"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
updated xl and added script for creating reduced ds
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results-new.xlsx
+++ b/Baseline-experimental-results-new.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rogier\Documents\Studie\HWR_own\HWR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Oosterhuis\Documents\GitHub\HWR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="new_results" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Dataset</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>16 ( 4 min, 10-fold, ROG))</t>
+  </si>
+  <si>
+    <t>Extended_Reduced</t>
   </si>
 </sst>
 </file>
@@ -170,11 +173,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000000%"/>
-    <numFmt numFmtId="165" formatCode="0.00000%"/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -212,20 +215,20 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,7 +324,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -383,7 +386,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -505,7 +508,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -627,7 +630,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -743,7 +746,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -862,7 +865,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -917,6 +920,9 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.9446</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75049999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -978,7 +984,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1100,7 +1106,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475003128"/>
@@ -1174,7 +1180,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475002800"/>
@@ -1216,7 +1222,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1246,7 +1252,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1504,7 +1510,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438729832"/>
@@ -1565,7 +1571,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438729504"/>
@@ -1607,7 +1613,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1637,7 +1643,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3107,39 +3113,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" customWidth="1"/>
+    <col min="18" max="18" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3173,7 +3179,7 @@
       <c r="W1" s="14"/>
       <c r="X1" s="14"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3241,7 +3247,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>91580</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3311,7 +3317,7 @@
         <v>22895</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3346,7 +3352,7 @@
         <v>27646</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3384,7 +3390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3397,7 +3403,7 @@
         <v>9.4514499999999946E-2</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ref="D7:V7" si="0">1-D8</f>
+        <f t="shared" ref="D7:F7" si="0">1-D8</f>
         <v>4.2100000000000026E-2</v>
       </c>
       <c r="E7" s="1">
@@ -3464,7 +3470,7 @@
       </c>
       <c r="V7" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.24950000000000006</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" si="1"/>
@@ -3475,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3520,11 +3526,14 @@
       <c r="U8" s="2">
         <v>0.63190000000000002</v>
       </c>
+      <c r="V8" s="2">
+        <v>0.75049999999999994</v>
+      </c>
       <c r="W8" s="2">
         <v>0.19650000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -3547,7 +3556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -3578,7 +3587,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -3597,7 +3606,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3614,7 +3623,10 @@
         <f>U8</f>
         <v>0.63190000000000002</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2">
+        <f>V8</f>
+        <v>0.75049999999999994</v>
+      </c>
       <c r="G13" s="2">
         <f>W8</f>
         <v>0.19650000000000001</v>
@@ -3622,9 +3634,14 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3646,17 +3663,17 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3673,7 +3690,7 @@
       </c>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3696,7 +3713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3712,7 +3729,7 @@
       <c r="G3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3727,7 +3744,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3742,7 +3759,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3757,7 +3774,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3772,7 +3789,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3787,7 +3804,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3802,7 +3819,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3817,7 +3834,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3832,7 +3849,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3847,7 +3864,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3877,7 +3894,7 @@
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -3907,7 +3924,7 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -3937,7 +3954,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3948,7 +3965,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3963,7 +3980,7 @@
       <c r="D19" s="9"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3978,7 +3995,7 @@
       <c r="D20" s="9"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
results baseline and 6conv no dropout
</commit_message>
<xml_diff>
--- a/Baseline-experimental-results-new.xlsx
+++ b/Baseline-experimental-results-new.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rogier\Documents\Studie\HWR_own\HWR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Oosterhuis\Documents\GitHub\HWR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="new_results" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t>Dataset</t>
   </si>
@@ -214,6 +214,27 @@
   </si>
   <si>
     <t>16 (t=3:21, PER)</t>
+  </si>
+  <si>
+    <t>base-CNN-nodrop</t>
+  </si>
+  <si>
+    <t>CNN_6conv-nodrop</t>
+  </si>
+  <si>
+    <t>CNN_6conv</t>
+  </si>
+  <si>
+    <t>22 (t=2.19, PER)</t>
+  </si>
+  <si>
+    <t>12 (10 min, PER)</t>
+  </si>
+  <si>
+    <t>6 (3 min, PER)</t>
+  </si>
+  <si>
+    <t>11 (67 min, PER)</t>
   </si>
 </sst>
 </file>
@@ -221,11 +242,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.000000%"/>
-    <numFmt numFmtId="165" formatCode="0.00000%"/>
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.000000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -263,22 +284,25 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,7 +399,7 @@
               <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -437,7 +461,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -565,7 +589,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -693,7 +717,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -818,7 +842,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -943,7 +967,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1071,7 +1095,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1157,7 +1181,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CNN_6conv_1</c:v>
+                  <c:v>CNN_6conv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1201,7 +1225,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-NL"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1332,7 +1356,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475003128"/>
@@ -1406,7 +1430,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="475002800"/>
@@ -1448,7 +1472,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1478,7 +1502,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1736,7 +1760,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438729832"/>
@@ -1797,7 +1821,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="438729504"/>
@@ -1839,7 +1863,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1869,7 +1893,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2970,7 +2994,7 @@
       <xdr:rowOff>137432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>283029</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>4082</xdr:rowOff>
@@ -3339,90 +3363,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF15"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.140625" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.7109375" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" customWidth="1"/>
+    <col min="20" max="20" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.109375" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="16.88671875" customWidth="1"/>
+    <col min="30" max="30" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
+    <col min="34" max="34" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="16" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="16" t="s">
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="14"/>
-      <c r="Z1" s="16" t="s">
-        <v>46</v>
-      </c>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="14"/>
       <c r="AA1" s="16"/>
       <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="15"/>
+      <c r="AD1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="15"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3442,76 +3473,88 @@
         <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
         <v>57</v>
       </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
       <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>57</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>29</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>39</v>
       </c>
-      <c r="R2" t="s">
-        <v>20</v>
-      </c>
-      <c r="S2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" t="s">
-        <v>31</v>
-      </c>
-      <c r="U2" t="s">
-        <v>57</v>
-      </c>
-      <c r="V2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>39</v>
-      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3536,29 +3579,29 @@
       <c r="H3">
         <v>21584</v>
       </c>
+      <c r="I3">
+        <v>21584</v>
+      </c>
       <c r="J3">
+        <v>21584</v>
+      </c>
+      <c r="L3">
         <v>220624</v>
       </c>
-      <c r="K3">
-        <v>196110</v>
-      </c>
-      <c r="N3">
-        <v>196110</v>
-      </c>
-      <c r="O3">
+      <c r="M3">
         <v>196110</v>
       </c>
       <c r="P3">
         <v>196110</v>
       </c>
+      <c r="Q3">
+        <v>196110</v>
+      </c>
       <c r="R3">
+        <v>196110</v>
+      </c>
+      <c r="T3">
         <v>127800</v>
-      </c>
-      <c r="S3">
-        <v>113600</v>
-      </c>
-      <c r="T3">
-        <v>113600</v>
       </c>
       <c r="U3">
         <v>113600</v>
@@ -3572,20 +3615,20 @@
       <c r="X3">
         <v>113600</v>
       </c>
+      <c r="Y3">
+        <v>113600</v>
+      </c>
       <c r="Z3">
+        <v>113600</v>
+      </c>
+      <c r="AA3">
+        <v>113600</v>
+      </c>
+      <c r="AB3">
+        <v>113600</v>
+      </c>
+      <c r="AD3">
         <v>101684</v>
-      </c>
-      <c r="AA3">
-        <v>90386</v>
-      </c>
-      <c r="AB3">
-        <v>90386</v>
-      </c>
-      <c r="AC3">
-        <v>90386</v>
-      </c>
-      <c r="AD3">
-        <v>90386</v>
       </c>
       <c r="AE3">
         <v>90386</v>
@@ -3593,8 +3636,20 @@
       <c r="AF3">
         <v>90386</v>
       </c>
+      <c r="AG3">
+        <v>90386</v>
+      </c>
+      <c r="AH3">
+        <v>90386</v>
+      </c>
+      <c r="AI3">
+        <v>90386</v>
+      </c>
+      <c r="AJ3">
+        <v>90386</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3619,29 +3674,29 @@
       <c r="H4">
         <v>5396</v>
       </c>
+      <c r="I4">
+        <v>5396</v>
+      </c>
       <c r="J4">
+        <v>5396</v>
+      </c>
+      <c r="L4">
         <v>24513</v>
       </c>
-      <c r="K4">
-        <v>49027</v>
-      </c>
-      <c r="N4">
-        <v>49027</v>
-      </c>
-      <c r="O4">
+      <c r="M4">
         <v>49027</v>
       </c>
       <c r="P4">
         <v>49027</v>
       </c>
+      <c r="Q4">
+        <v>49027</v>
+      </c>
       <c r="R4">
+        <v>49027</v>
+      </c>
+      <c r="T4">
         <v>14200</v>
-      </c>
-      <c r="S4">
-        <v>28400</v>
-      </c>
-      <c r="T4">
-        <v>28400</v>
       </c>
       <c r="U4">
         <v>28400</v>
@@ -3655,20 +3710,20 @@
       <c r="X4">
         <v>28400</v>
       </c>
+      <c r="Y4">
+        <v>28400</v>
+      </c>
       <c r="Z4">
+        <v>28400</v>
+      </c>
+      <c r="AA4">
+        <v>28400</v>
+      </c>
+      <c r="AB4">
+        <v>28400</v>
+      </c>
+      <c r="AD4">
         <v>11298</v>
-      </c>
-      <c r="AA4">
-        <v>22596</v>
-      </c>
-      <c r="AB4">
-        <v>22596</v>
-      </c>
-      <c r="AC4">
-        <v>22596</v>
-      </c>
-      <c r="AD4">
-        <v>22596</v>
       </c>
       <c r="AE4">
         <v>22596</v>
@@ -3676,8 +3731,20 @@
       <c r="AF4">
         <v>22596</v>
       </c>
+      <c r="AG4">
+        <v>22596</v>
+      </c>
+      <c r="AH4">
+        <v>22596</v>
+      </c>
+      <c r="AI4">
+        <v>22596</v>
+      </c>
+      <c r="AJ4">
+        <v>22596</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3702,26 +3769,26 @@
       <c r="H5">
         <v>589</v>
       </c>
+      <c r="I5">
+        <v>589</v>
+      </c>
       <c r="J5">
         <v>589</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>589</v>
       </c>
-      <c r="N5">
-        <v>589</v>
-      </c>
-      <c r="O5">
+      <c r="M5">
         <v>589</v>
       </c>
       <c r="P5">
         <v>589</v>
       </c>
+      <c r="Q5">
+        <v>589</v>
+      </c>
       <c r="R5">
-        <v>27646</v>
-      </c>
-      <c r="S5">
-        <v>27646</v>
+        <v>589</v>
       </c>
       <c r="T5">
         <v>27646</v>
@@ -3738,17 +3805,17 @@
       <c r="X5">
         <v>27646</v>
       </c>
+      <c r="Y5">
+        <v>27646</v>
+      </c>
       <c r="Z5">
-        <v>13083</v>
+        <v>27646</v>
       </c>
       <c r="AA5">
-        <v>13083</v>
+        <v>27646</v>
       </c>
       <c r="AB5">
-        <v>13083</v>
-      </c>
-      <c r="AC5">
-        <v>13083</v>
+        <v>27646</v>
       </c>
       <c r="AD5">
         <v>13083</v>
@@ -3759,8 +3826,20 @@
       <c r="AF5">
         <v>13083</v>
       </c>
+      <c r="AG5">
+        <v>13083</v>
+      </c>
+      <c r="AH5">
+        <v>13083</v>
+      </c>
+      <c r="AI5">
+        <v>13083</v>
+      </c>
+      <c r="AJ5">
+        <v>13083</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3785,65 +3864,77 @@
       <c r="H6" t="s">
         <v>58</v>
       </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
       <c r="J6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
         <v>43</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>25</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>54</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>55</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>56</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>42</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>26</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>48</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>60</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>61</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>62</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>41</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD6" t="s">
         <v>51</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AE6" t="s">
         <v>47</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AF6" t="s">
         <v>52</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AG6" t="s">
         <v>59</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AH6" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AI6" t="s">
         <v>53</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AJ6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3872,97 +3963,113 @@
         <v>3.9300000000000002E-2</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7:X7" si="1">1-H8</f>
+        <f t="shared" ref="H7:Z7" si="1">1-H8</f>
         <v>3.8000000000000034E-2</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="2">
+        <f>1-I8</f>
+        <v>0.10209999999999997</v>
+      </c>
       <c r="J7" s="1">
+        <f>1-J8</f>
+        <v>5.3200000000000025E-2</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
         <f t="shared" si="1"/>
         <v>5.8199999999999918E-2</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <f t="shared" si="1"/>
         <v>1.315999999999995E-2</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M7" s="1">
-        <f>1-M8</f>
+      <c r="O7" s="1">
+        <f>1-O8</f>
         <v>1</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <f t="shared" si="1"/>
         <v>7.6000000000000512E-3</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <f t="shared" si="1"/>
         <v>8.0999999999999961E-3</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <f t="shared" si="1"/>
         <v>1.8000000000000016E-2</v>
       </c>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1">
+      <c r="S7" s="1"/>
+      <c r="T7" s="1">
         <f t="shared" si="1"/>
         <v>0.91739999999999999</v>
       </c>
-      <c r="S7" s="1">
+      <c r="U7" s="1">
         <f t="shared" si="1"/>
         <v>0.56950000000000001</v>
       </c>
-      <c r="T7" s="1">
+      <c r="V7" s="1">
         <f t="shared" si="1"/>
         <v>0.2419</v>
       </c>
-      <c r="U7" s="1">
-        <f>1-U8</f>
+      <c r="W7" s="1">
+        <f>1-W8</f>
         <v>0.18910000000000005</v>
       </c>
-      <c r="V7" s="1">
+      <c r="X7" s="1">
         <f t="shared" si="1"/>
         <v>0.36809999999999998</v>
       </c>
-      <c r="W7" s="1">
+      <c r="Y7" s="1">
         <f t="shared" si="1"/>
         <v>0.24950000000000006</v>
       </c>
-      <c r="X7" s="1">
+      <c r="Z7" s="1">
         <f t="shared" si="1"/>
         <v>0.80349999999999999</v>
       </c>
-      <c r="Z7" s="2">
-        <f t="shared" ref="Z7:AF7" si="2">1-Z8</f>
+      <c r="AA7" s="1">
+        <f>1-AA8</f>
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="AB7" s="1">
+        <f>1-AB8</f>
+        <v>0.27390000000000003</v>
+      </c>
+      <c r="AD7" s="2">
+        <f t="shared" ref="AD7:AJ7" si="2">1-AD8</f>
         <v>0.8901</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AE7" s="2">
         <f t="shared" si="2"/>
         <v>0.33750000000000002</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AF7" s="2">
         <f t="shared" si="2"/>
         <v>0.21550000000000002</v>
       </c>
-      <c r="AC7" s="2">
-        <f>1-AC8</f>
+      <c r="AG7" s="2">
+        <f>1-AG8</f>
         <v>9.209999999999996E-2</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AH7" s="2">
         <f t="shared" si="2"/>
         <v>0.16469999999999996</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AI7" s="2">
         <f t="shared" si="2"/>
         <v>0.13900000000000001</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AJ7" s="2">
         <f t="shared" si="2"/>
         <v>0.5726</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3987,69 +4094,81 @@
       <c r="H8" s="1">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1">
+        <v>0.89790000000000003</v>
+      </c>
       <c r="J8" s="1">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1">
         <v>0.94180000000000008</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
         <v>0.98684000000000005</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1">
         <v>0.99239999999999995</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <v>0.9919</v>
       </c>
-      <c r="P8" s="1">
+      <c r="R8" s="1">
         <v>0.98199999999999998</v>
       </c>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2">
+      <c r="S8" s="1"/>
+      <c r="T8" s="2">
         <v>8.2600000000000007E-2</v>
       </c>
-      <c r="S8" s="1">
+      <c r="U8" s="1">
         <v>0.43049999999999999</v>
       </c>
-      <c r="T8" s="2">
+      <c r="V8" s="2">
         <v>0.7581</v>
       </c>
-      <c r="U8" s="2">
+      <c r="W8" s="2">
         <v>0.81089999999999995</v>
       </c>
-      <c r="V8" s="2">
+      <c r="X8" s="2">
         <v>0.63190000000000002</v>
       </c>
-      <c r="W8" s="2">
+      <c r="Y8" s="2">
         <v>0.75049999999999994</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Z8" s="2">
         <v>0.19650000000000001</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AA8" s="2">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0.72609999999999997</v>
+      </c>
+      <c r="AD8" s="2">
         <v>0.1099</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AE8" s="2">
         <v>0.66249999999999998</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AF8" s="2">
         <v>0.78449999999999998</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AG8" s="2">
         <v>0.90790000000000004</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AH8" s="2">
         <v>0.83530000000000004</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AI8" s="2">
         <v>0.86099999999999999</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AJ8" s="2">
         <v>0.4274</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -4069,10 +4188,16 @@
         <v>30</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>65</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -4104,40 +4229,50 @@
         <f>G8</f>
         <v>0.9607</v>
       </c>
+      <c r="I11" s="2">
+        <f>I8</f>
+        <v>0.89790000000000003</v>
+      </c>
+      <c r="J11" s="2">
+        <f>J8</f>
+        <v>0.94679999999999997</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <f>J8</f>
+        <f>L8</f>
         <v>0.94180000000000008</v>
       </c>
       <c r="C12" s="2">
-        <f>K8</f>
+        <f>M8</f>
         <v>0.98684000000000005</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <f>N8</f>
+        <f>P8</f>
         <v>0.99239999999999995</v>
       </c>
       <c r="G12" s="2">
-        <f>O8</f>
+        <f>Q8</f>
         <v>0.9919</v>
       </c>
       <c r="H12" s="2">
-        <f>P8</f>
+        <f>R8</f>
         <v>0.98199999999999998</v>
       </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" ref="B13:D13" si="4">R8</f>
+        <f t="shared" ref="B13:D13" si="4">T8</f>
         <v>8.2600000000000007E-2</v>
       </c>
       <c r="C13" s="2">
@@ -4149,28 +4284,36 @@
         <v>0.7581</v>
       </c>
       <c r="E13" s="2">
-        <f>U8</f>
+        <f>W8</f>
         <v>0.81089999999999995</v>
       </c>
       <c r="F13" s="2">
-        <f>V8</f>
+        <f>X8</f>
         <v>0.63190000000000002</v>
       </c>
       <c r="G13" s="2">
-        <f>W8</f>
+        <f>Y8</f>
         <v>0.75049999999999994</v>
       </c>
       <c r="H13" s="2">
-        <f>X8</f>
+        <f>Z8</f>
         <v>0.19650000000000001</v>
       </c>
+      <c r="I13" s="2">
+        <f>AA8</f>
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="J13" s="2">
+        <f>AB8</f>
+        <v>0.72609999999999997</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" ref="B14:D14" si="5">Z8</f>
+        <f t="shared" ref="B14:D14" si="5">AD8</f>
         <v>0.1099</v>
       </c>
       <c r="C14" s="2">
@@ -4182,33 +4325,35 @@
         <v>0.78449999999999998</v>
       </c>
       <c r="E14" s="2">
-        <f>AC8</f>
+        <f>AG8</f>
         <v>0.90790000000000004</v>
       </c>
       <c r="F14" s="2">
-        <f>AD8</f>
+        <f>AH8</f>
         <v>0.83530000000000004</v>
       </c>
       <c r="G14" s="2">
-        <f>AE8</f>
+        <f>AI8</f>
         <v>0.86099999999999999</v>
       </c>
       <c r="H14" s="2">
-        <f>AF8</f>
+        <f>AJ8</f>
         <v>0.4274</v>
       </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="T1:Y1"/>
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="AD1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4223,34 +4368,34 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -4273,7 +4418,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4289,7 +4434,7 @@
       <c r="G3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4304,7 +4449,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4319,7 +4464,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4334,7 +4479,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4349,7 +4494,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4364,7 +4509,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4379,7 +4524,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4394,7 +4539,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4409,7 +4554,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4424,7 +4569,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4454,7 +4599,7 @@
       </c>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -4484,7 +4629,7 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -4514,7 +4659,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -4525,7 +4670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -4540,7 +4685,7 @@
       <c r="D19" s="9"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -4555,7 +4700,7 @@
       <c r="D20" s="9"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>

</xml_diff>